<commit_message>
Handle all parameter values
</commit_message>
<xml_diff>
--- a/Examples/HelpExamples.xlsx
+++ b/Examples/HelpExamples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Excel-DNA\XFunctions\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2160674F-6F73-4345-86EC-98B3DC33C335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91C19E-236E-4DAB-9110-C60247C92E6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="2280" windowWidth="21600" windowHeight="11160" xr2:uid="{D5122D25-816F-4AEC-A929-CABFF95EF948}"/>
+    <workbookView xWindow="2280" yWindow="3240" windowWidth="21600" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{D5122D25-816F-4AEC-A929-CABFF95EF948}"/>
   </bookViews>
   <sheets>
     <sheet name="XLOOKUP 1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="XMATCH 4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -763,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105464BA-F696-4614-9117-A2CA6E66FBB5}">
   <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -923,7 +924,7 @@
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,9 +958,9 @@
       <c r="E2" s="7">
         <v>46523</v>
       </c>
-      <c r="F2" s="4" t="e" cm="1">
-        <f t="array" ref="F2">_xll.XLOOKUP(E2,C2:C7,B2:B7)</f>
-        <v>#N/A</v>
+      <c r="F2" s="4" cm="1">
+        <f t="array" ref="F2">_xll.XLOOKUP(E2,C2:C7,B2:B7,1,1)</f>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -1430,7 +1431,7 @@
   <dimension ref="C2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1489,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,9 +1531,9 @@
       <c r="E4" t="s">
         <v>77</v>
       </c>
-      <c r="F4" t="e" cm="1">
-        <f t="array" ref="F4">_xll.XMATCH(F2, C3:C9, -1)</f>
-        <v>#N/A</v>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">_xll.XMATCH(F2, C3:C9, 1)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1829,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7511B1-04C3-4510-9876-9AB4F8DA456D}">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1848,9 +1849,9 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="e" cm="1">
+      <c r="B3" cm="1">
         <f t="array" ref="B3">_xll.XMATCH(4.5,{5,4,3,2,1},1)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>79</v>

</xml_diff>